<commit_message>
Commit for latest change
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/BGHS_PreAdmissionData.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/BGHS_PreAdmissionData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13515" windowHeight="6330" firstSheet="13" activeTab="14"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13515" windowHeight="6330" firstSheet="22" activeTab="22"/>
   </bookViews>
   <sheets>
     <sheet name="BGHS_StudentDetailsData" sheetId="1" r:id="rId1"/>
@@ -24,13 +24,20 @@
     <sheet name="BGHS_OralTestScheduleData" sheetId="16" r:id="rId15"/>
     <sheet name="BGHS_ScheduleNameData" sheetId="17" r:id="rId16"/>
     <sheet name="BGHS_searchExistingStuNameData" sheetId="18" r:id="rId17"/>
+    <sheet name="search_ScheduleNameData" sheetId="20" r:id="rId18"/>
+    <sheet name="WrittenTestFormData" sheetId="22" r:id="rId19"/>
+    <sheet name="TransferPreAdmToAdmData" sheetId="23" r:id="rId20"/>
+    <sheet name="search_transferStudent" sheetId="24" r:id="rId21"/>
+    <sheet name="YearWiseStudentCountData" sheetId="25" r:id="rId22"/>
+    <sheet name="Search_UserNameYearBetween" sheetId="26" r:id="rId23"/>
+    <sheet name="Search_regFilledApplForm" sheetId="27" r:id="rId24"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="148">
   <si>
     <t>FirstName</t>
   </si>
@@ -429,18 +436,91 @@
   </si>
   <si>
     <t>02-02-2018</t>
+  </si>
+  <si>
+    <t>FromHr</t>
+  </si>
+  <si>
+    <t>FromMin</t>
+  </si>
+  <si>
+    <t>ToHr</t>
+  </si>
+  <si>
+    <t>ToMin</t>
+  </si>
+  <si>
+    <t>Visual Recognition</t>
+  </si>
+  <si>
+    <t>AnyOne Available</t>
+  </si>
+  <si>
+    <t>Written Test For Admission</t>
+  </si>
+  <si>
+    <t>Vaps Written Test</t>
+  </si>
+  <si>
+    <t>Academic Year</t>
+  </si>
+  <si>
+    <t>New PN</t>
+  </si>
+  <si>
+    <t>2018-2019</t>
+  </si>
+  <si>
+    <t>Registration Number</t>
+  </si>
+  <si>
+    <t>1271</t>
+  </si>
+  <si>
+    <t>BCEHS</t>
+  </si>
+  <si>
+    <t>UserName</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="7">
+  <fonts count="13">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -483,6 +563,20 @@
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -503,38 +597,61 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1197,8 +1314,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1365,6 +1482,117 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="11" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="13" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="F1" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="H1" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="I1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="E2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>127</v>
+      </c>
+      <c r="G2" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="H2" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D2"/>
@@ -1410,6 +1638,176 @@
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="18.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="18" t="s">
+        <v>146</v>
+      </c>
+      <c r="B2" s="17" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="13.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Commit for marks Entry
</commit_message>
<xml_diff>
--- a/src/main/java/com/vapsTechnosoft/IVRM/data/BGHS_PreAdmissionData.xlsx
+++ b/src/main/java/com/vapsTechnosoft/IVRM/data/BGHS_PreAdmissionData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2520" windowWidth="13515" windowHeight="6330" firstSheet="22" activeTab="22"/>
+    <workbookView xWindow="0" yWindow="2520" windowWidth="13515" windowHeight="6330" firstSheet="28" activeTab="30"/>
   </bookViews>
   <sheets>
     <sheet name="BGHS_StudentDetailsData" sheetId="1" r:id="rId1"/>
@@ -31,13 +31,20 @@
     <sheet name="YearWiseStudentCountData" sheetId="25" r:id="rId22"/>
     <sheet name="Search_UserNameYearBetween" sheetId="26" r:id="rId23"/>
     <sheet name="Search_regFilledApplForm" sheetId="27" r:id="rId24"/>
+    <sheet name="Application_StatusData" sheetId="28" r:id="rId25"/>
+    <sheet name="Admission_StatusData" sheetId="29" r:id="rId26"/>
+    <sheet name="UpdateStatusAll" sheetId="30" r:id="rId27"/>
+    <sheet name="Search_Student_Application" sheetId="31" r:id="rId28"/>
+    <sheet name="StatusRemarks_appStatus" sheetId="32" r:id="rId29"/>
+    <sheet name="Status_EmailSmSDetails" sheetId="33" r:id="rId30"/>
+    <sheet name="Search_Student_Admission" sheetId="34" r:id="rId31"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="165">
   <si>
     <t>FirstName</t>
   </si>
@@ -481,18 +488,76 @@
   </si>
   <si>
     <t>UserName</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>PN</t>
+  </si>
+  <si>
+    <t>APP WAITING</t>
+  </si>
+  <si>
+    <t>INPROGRESS</t>
+  </si>
+  <si>
+    <t>APP ACCEPTED</t>
+  </si>
+  <si>
+    <t>ANUSHKA GAGAN KARDE</t>
+  </si>
+  <si>
+    <t>Student status updated</t>
+  </si>
+  <si>
+    <t>EmailSubject</t>
+  </si>
+  <si>
+    <t>EmailHeader</t>
+  </si>
+  <si>
+    <t>EmailMessage</t>
+  </si>
+  <si>
+    <t>EmailFoother</t>
+  </si>
+  <si>
+    <t>SmSContent</t>
+  </si>
+  <si>
+    <t>Your Child Admission Status Update on Portal</t>
+  </si>
+  <si>
+    <t>Thank You</t>
+  </si>
+  <si>
+    <t>Dear Parent</t>
+  </si>
+  <si>
+    <t>Status Update</t>
+  </si>
+  <si>
+    <t>DAIVANSH C</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="13">
+  <fonts count="15">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -577,6 +642,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF222222"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -597,61 +669,68 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="top"/>
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1755,7 +1834,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -1811,6 +1890,203 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>150</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="D1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="C2" s="19" t="s">
+        <v>151</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="14.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="19" t="s">
+        <v>152</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H19" sqref="H19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="22" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="21" t="s">
+        <v>154</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G2"/>
@@ -1869,6 +2145,102 @@
     </row>
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:F2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="41.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="20" t="s">
+        <v>155</v>
+      </c>
+      <c r="B1" s="20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C1" s="20" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="E1" s="20" t="s">
+        <v>159</v>
+      </c>
+      <c r="F1" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="20" t="s">
+        <v>163</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>162</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" s="20" t="s">
+        <v>161</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>160</v>
+      </c>
+      <c r="F2" s="20" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B2" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 

</xml_diff>